<commit_message>
Excel file into ProbandoLecturaFichero.java
</commit_message>
<xml_diff>
--- a/Java/restassuredsample/testData/UserData.xlsx
+++ b/Java/restassuredsample/testData/UserData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lourd\Documents\Lenovo_D\Lourdes\practicando\Practices\Java\restassuredsample\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C37ECCA-4A40-4532-B42B-4F43B7E339BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E020CB93-649B-4C3B-BCBD-386032662B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -133,7 +133,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyProtection="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -455,7 +455,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="179" zoomScaleNormal="179" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H1" sqref="H1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>